<commit_message>
add example of plotting curve
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="1276">
   <si>
     <t>name</t>
   </si>
@@ -1507,6 +1507,549 @@
   </si>
   <si>
     <t>length_humerus_R</t>
+  </si>
+  <si>
+    <t>mean_velocity_ankle_L</t>
+  </si>
+  <si>
+    <t>mean_velocity_ankle_R</t>
+  </si>
+  <si>
+    <t>mean_velocity_knee_L</t>
+  </si>
+  <si>
+    <t>mean_velocity_knee_R</t>
+  </si>
+  <si>
+    <t>mean_velocity_bladder</t>
+  </si>
+  <si>
+    <t>mean_velocity_elbow_L</t>
+  </si>
+  <si>
+    <t>mean_velocity_elbow_R</t>
+  </si>
+  <si>
+    <t>mean_velocity_eye_L</t>
+  </si>
+  <si>
+    <t>mean_velocity_eye_R</t>
+  </si>
+  <si>
+    <t>mean_velocity_hip_L</t>
+  </si>
+  <si>
+    <t>mean_velocity_hip_R</t>
+  </si>
+  <si>
+    <t>mean_velocity_shoulder_L</t>
+  </si>
+  <si>
+    <t>mean_velocity_shoulder_R</t>
+  </si>
+  <si>
+    <t>mean_velocity_wrist_L</t>
+  </si>
+  <si>
+    <t>mean_velocity_wrist_R</t>
+  </si>
+  <si>
+    <t>std_velocity_ankle_L</t>
+  </si>
+  <si>
+    <t>std_velocity_ankle_R</t>
+  </si>
+  <si>
+    <t>std_velocity_knee_L</t>
+  </si>
+  <si>
+    <t>std_velocity_knee_R</t>
+  </si>
+  <si>
+    <t>std_velocity_bladder</t>
+  </si>
+  <si>
+    <t>std_velocity_elbow_L</t>
+  </si>
+  <si>
+    <t>std_velocity_elbow_R</t>
+  </si>
+  <si>
+    <t>std_velocity_eye_L</t>
+  </si>
+  <si>
+    <t>std_velocity_eye_R</t>
+  </si>
+  <si>
+    <t>std_velocity_hip_L</t>
+  </si>
+  <si>
+    <t>std_velocity_hip_R</t>
+  </si>
+  <si>
+    <t>std_velocity_shoulder_L</t>
+  </si>
+  <si>
+    <t>std_velocity_shoulder_R</t>
+  </si>
+  <si>
+    <t>std_velocity_wrist_L</t>
+  </si>
+  <si>
+    <t>std_velocity_wrist_R</t>
+  </si>
+  <si>
+    <t>avg_angle_knee_L</t>
+  </si>
+  <si>
+    <t>avg_angle_knee_R</t>
+  </si>
+  <si>
+    <t>avg_angle_elbow_L</t>
+  </si>
+  <si>
+    <t>avg_angle_elbow_R</t>
+  </si>
+  <si>
+    <t>std_angle_knee_L</t>
+  </si>
+  <si>
+    <t>std_angle_knee_R</t>
+  </si>
+  <si>
+    <t>std_angle_elbow_L</t>
+  </si>
+  <si>
+    <t>std_angle_elbow_R</t>
+  </si>
+  <si>
+    <t>avg_angle_velocity_knee_L</t>
+  </si>
+  <si>
+    <t>avg_angle_velocity_knee_R</t>
+  </si>
+  <si>
+    <t>avg_angle_velocity_elbow_L</t>
+  </si>
+  <si>
+    <t>avg_angle_velocity_elbow_R</t>
+  </si>
+  <si>
+    <t>std_angle_velocity_knee_L</t>
+  </si>
+  <si>
+    <t>std_angle_velocity_knee_R</t>
+  </si>
+  <si>
+    <t>std_angle_velocity_elbow_L</t>
+  </si>
+  <si>
+    <t>std_angle_velocity_elbow_R</t>
+  </si>
+  <si>
+    <t>avg_angle_acceleration_knee_L</t>
+  </si>
+  <si>
+    <t>avg_angle_acceleration_knee_R</t>
+  </si>
+  <si>
+    <t>avg_angle_acceleration_elbow_L</t>
+  </si>
+  <si>
+    <t>avg_angle_acceleration_elbow_R</t>
+  </si>
+  <si>
+    <t>std_angle_acceleration_knee_L</t>
+  </si>
+  <si>
+    <t>std_angle_acceleration_knee_R</t>
+  </si>
+  <si>
+    <t>std_angle_acceleration_elbow_L</t>
+  </si>
+  <si>
+    <t>std_angle_acceleration_elbow_R</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>010918L</t>
+  </si>
+  <si>
+    <t>010918S</t>
+  </si>
+  <si>
+    <t>013018L</t>
+  </si>
+  <si>
+    <t>013018S</t>
+  </si>
+  <si>
+    <t>013118L</t>
+  </si>
+  <si>
+    <t>013118S</t>
+  </si>
+  <si>
+    <t>021218L</t>
+  </si>
+  <si>
+    <t>021218S</t>
+  </si>
+  <si>
+    <t>022318L</t>
+  </si>
+  <si>
+    <t>022318S</t>
+  </si>
+  <si>
+    <t>022618</t>
+  </si>
+  <si>
+    <t>031317L</t>
+  </si>
+  <si>
+    <t>031317T</t>
+  </si>
+  <si>
+    <t>031615</t>
+  </si>
+  <si>
+    <t>031616</t>
+  </si>
+  <si>
+    <t>032217</t>
+  </si>
+  <si>
+    <t>032318a</t>
+  </si>
+  <si>
+    <t>032318b</t>
+  </si>
+  <si>
+    <t>032318c</t>
+  </si>
+  <si>
+    <t>032318d</t>
+  </si>
+  <si>
+    <t>032818</t>
+  </si>
+  <si>
+    <t>040218</t>
+  </si>
+  <si>
+    <t>040417</t>
+  </si>
+  <si>
+    <t>040716</t>
+  </si>
+  <si>
+    <t>041017</t>
+  </si>
+  <si>
+    <t>041318L</t>
+  </si>
+  <si>
+    <t>041818</t>
+  </si>
+  <si>
+    <t>043015</t>
+  </si>
+  <si>
+    <t>050318L</t>
+  </si>
+  <si>
+    <t>051718L</t>
+  </si>
+  <si>
+    <t>051718S</t>
+  </si>
+  <si>
+    <t>051817</t>
+  </si>
+  <si>
+    <t>052218L</t>
+  </si>
+  <si>
+    <t>052218S</t>
+  </si>
+  <si>
+    <t>052418L</t>
+  </si>
+  <si>
+    <t>052418S</t>
+  </si>
+  <si>
+    <t>052516</t>
+  </si>
+  <si>
+    <t>053017</t>
+  </si>
+  <si>
+    <t>053117L</t>
+  </si>
+  <si>
+    <t>053117S</t>
+  </si>
+  <si>
+    <t>061217</t>
+  </si>
+  <si>
+    <t>062117</t>
+  </si>
+  <si>
+    <t>062817L</t>
+  </si>
+  <si>
+    <t>062817S</t>
+  </si>
+  <si>
+    <t>071218</t>
+  </si>
+  <si>
+    <t>071717L</t>
+  </si>
+  <si>
+    <t>071717S</t>
+  </si>
+  <si>
+    <t>072017L</t>
+  </si>
+  <si>
+    <t>072017S</t>
+  </si>
+  <si>
+    <t>080217</t>
+  </si>
+  <si>
+    <t>082117L</t>
+  </si>
+  <si>
+    <t>082117S</t>
+  </si>
+  <si>
+    <t>082517L</t>
+  </si>
+  <si>
+    <t>082917a</t>
+  </si>
+  <si>
+    <t>082917b</t>
+  </si>
+  <si>
+    <t>083017L</t>
+  </si>
+  <si>
+    <t>083017S</t>
+  </si>
+  <si>
+    <t>083115</t>
+  </si>
+  <si>
+    <t>090517L</t>
+  </si>
+  <si>
+    <t>091917L</t>
+  </si>
+  <si>
+    <t>091917S</t>
+  </si>
+  <si>
+    <t>092117L</t>
+  </si>
+  <si>
+    <t>092117S</t>
+  </si>
+  <si>
+    <t>092817L</t>
+  </si>
+  <si>
+    <t>100317L</t>
+  </si>
+  <si>
+    <t>100317S</t>
+  </si>
+  <si>
+    <t>101317</t>
+  </si>
+  <si>
+    <t>102617</t>
+  </si>
+  <si>
+    <t>103017a</t>
+  </si>
+  <si>
+    <t>103017b</t>
+  </si>
+  <si>
+    <t>110214</t>
+  </si>
+  <si>
+    <t>110217L</t>
+  </si>
+  <si>
+    <t>111017L</t>
+  </si>
+  <si>
+    <t>111017S</t>
+  </si>
+  <si>
+    <t>120717</t>
+  </si>
+  <si>
+    <t>121517a</t>
+  </si>
+  <si>
+    <t>121517b</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>GA_week</t>
+  </si>
+  <si>
+    <t>GA_day</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_ankle_L</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_ankle_R</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_knee_L</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_knee_R</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_bladder</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_elbow_L</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_elbow_R</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_eye_L</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_eye_R</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_hip_L</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_hip_R</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_shoulder_L</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_shoulder_R</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_wrist_L</t>
+  </si>
+  <si>
+    <t>movement_time_absolute_wrist_R</t>
+  </si>
+  <si>
+    <t>movement_time_relative_ankle_L</t>
+  </si>
+  <si>
+    <t>movement_time_relative_ankle_R</t>
+  </si>
+  <si>
+    <t>movement_time_relative_knee_L</t>
+  </si>
+  <si>
+    <t>movement_time_relative_knee_R</t>
+  </si>
+  <si>
+    <t>movement_time_relative_bladder</t>
+  </si>
+  <si>
+    <t>movement_time_relative_elbow_L</t>
+  </si>
+  <si>
+    <t>movement_time_relative_elbow_R</t>
+  </si>
+  <si>
+    <t>movement_time_relative_eye_L</t>
+  </si>
+  <si>
+    <t>movement_time_relative_eye_R</t>
+  </si>
+  <si>
+    <t>movement_time_relative_hip_L</t>
+  </si>
+  <si>
+    <t>movement_time_relative_hip_R</t>
+  </si>
+  <si>
+    <t>movement_time_relative_shoulder_L</t>
+  </si>
+  <si>
+    <t>movement_time_relative_shoulder_R</t>
+  </si>
+  <si>
+    <t>movement_time_relative_wrist_L</t>
+  </si>
+  <si>
+    <t>movement_time_relative_wrist_R</t>
+  </si>
+  <si>
+    <t>avg_length_tibia_L</t>
+  </si>
+  <si>
+    <t>avg_length_tibia_R</t>
+  </si>
+  <si>
+    <t>avg_length_femur_L</t>
+  </si>
+  <si>
+    <t>avg_length_femur_R</t>
+  </si>
+  <si>
+    <t>avg_length_radius_L</t>
+  </si>
+  <si>
+    <t>avg_length_radius_R</t>
+  </si>
+  <si>
+    <t>avg_length_humerus_L</t>
+  </si>
+  <si>
+    <t>avg_length_humerus_R</t>
+  </si>
+  <si>
+    <t>std_length_tibia_L</t>
+  </si>
+  <si>
+    <t>std_length_tibia_R</t>
+  </si>
+  <si>
+    <t>std_length_femur_L</t>
+  </si>
+  <si>
+    <t>std_length_femur_R</t>
+  </si>
+  <si>
+    <t>std_length_radius_L</t>
+  </si>
+  <si>
+    <t>std_length_radius_R</t>
+  </si>
+  <si>
+    <t>std_length_humerus_L</t>
+  </si>
+  <si>
+    <t>std_length_humerus_R</t>
   </si>
   <si>
     <t>mean_velocity_ankle_L</t>
@@ -3318,7 +3861,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -3333,11 +3876,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -3346,6 +3890,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3358,429 +3903,429 @@
   <dimension ref="A1:CZ78"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.15625" customWidth="true"/>
+    <col min="1" max="1" width="8.28515625" customWidth="true"/>
     <col min="2" max="2" width="11.7109375" customWidth="true"/>
-    <col min="3" max="3" width="8.82421875" customWidth="true"/>
-    <col min="4" max="4" width="7.37890625" customWidth="true"/>
-    <col min="5" max="5" width="29.82421875" customWidth="true"/>
-    <col min="6" max="6" width="30.046875" customWidth="true"/>
-    <col min="7" max="7" width="29.37890625" customWidth="true"/>
-    <col min="8" max="8" width="29.6015625" customWidth="true"/>
-    <col min="9" max="9" width="29.7109375" customWidth="true"/>
-    <col min="10" max="10" width="30.48828125" customWidth="true"/>
-    <col min="11" max="11" width="30.7109375" customWidth="true"/>
-    <col min="12" max="12" width="28.37890625" customWidth="true"/>
-    <col min="13" max="13" width="28.6015625" customWidth="true"/>
-    <col min="14" max="14" width="27.93359375" customWidth="true"/>
-    <col min="15" max="15" width="28.15625" customWidth="true"/>
-    <col min="16" max="16" width="32.48828125" customWidth="true"/>
-    <col min="17" max="17" width="32.7109375" customWidth="true"/>
-    <col min="18" max="18" width="29.48828125" customWidth="true"/>
-    <col min="19" max="19" width="29.7109375" customWidth="true"/>
-    <col min="20" max="20" width="28.93359375" customWidth="true"/>
-    <col min="21" max="21" width="29.15625" customWidth="true"/>
-    <col min="22" max="22" width="28.48828125" customWidth="true"/>
-    <col min="23" max="23" width="28.7109375" customWidth="true"/>
-    <col min="24" max="24" width="28.82421875" customWidth="true"/>
-    <col min="25" max="25" width="29.6015625" customWidth="true"/>
-    <col min="26" max="26" width="29.82421875" customWidth="true"/>
-    <col min="27" max="27" width="27.48828125" customWidth="true"/>
-    <col min="28" max="28" width="27.7109375" customWidth="true"/>
-    <col min="29" max="29" width="27.046875" customWidth="true"/>
-    <col min="30" max="30" width="27.26953125" customWidth="true"/>
-    <col min="31" max="31" width="31.6015625" customWidth="true"/>
-    <col min="32" max="32" width="31.82421875" customWidth="true"/>
-    <col min="33" max="33" width="28.6015625" customWidth="true"/>
-    <col min="34" max="34" width="28.82421875" customWidth="true"/>
-    <col min="35" max="35" width="16.37890625" customWidth="true"/>
-    <col min="36" max="36" width="16.6015625" customWidth="true"/>
-    <col min="37" max="37" width="17.7109375" customWidth="true"/>
-    <col min="38" max="38" width="17.93359375" customWidth="true"/>
-    <col min="39" max="39" width="17.7109375" customWidth="true"/>
-    <col min="40" max="40" width="17.93359375" customWidth="true"/>
-    <col min="41" max="41" width="19.82421875" customWidth="true"/>
-    <col min="42" max="42" width="20.046875" customWidth="true"/>
-    <col min="43" max="43" width="16.046875" customWidth="true"/>
-    <col min="44" max="44" width="16.26953125" customWidth="true"/>
-    <col min="45" max="45" width="17.37890625" customWidth="true"/>
-    <col min="46" max="46" width="17.6015625" customWidth="true"/>
-    <col min="47" max="47" width="17.37890625" customWidth="true"/>
-    <col min="48" max="48" width="17.6015625" customWidth="true"/>
-    <col min="49" max="49" width="19.48828125" customWidth="true"/>
-    <col min="50" max="50" width="19.7109375" customWidth="true"/>
-    <col min="51" max="51" width="20.26953125" customWidth="true"/>
-    <col min="52" max="52" width="20.48828125" customWidth="true"/>
-    <col min="53" max="53" width="19.82421875" customWidth="true"/>
-    <col min="54" max="54" width="20.046875" customWidth="true"/>
-    <col min="55" max="55" width="20.15625" customWidth="true"/>
-    <col min="56" max="56" width="20.93359375" customWidth="true"/>
-    <col min="57" max="57" width="21.15625" customWidth="true"/>
-    <col min="58" max="58" width="18.82421875" customWidth="true"/>
-    <col min="59" max="59" width="19.046875" customWidth="true"/>
-    <col min="60" max="60" width="18.37890625" customWidth="true"/>
-    <col min="61" max="61" width="18.6015625" customWidth="true"/>
-    <col min="62" max="62" width="22.93359375" customWidth="true"/>
-    <col min="63" max="63" width="23.15625" customWidth="true"/>
-    <col min="64" max="64" width="19.93359375" customWidth="true"/>
-    <col min="65" max="65" width="20.15625" customWidth="true"/>
-    <col min="66" max="66" width="18.15625" customWidth="true"/>
-    <col min="67" max="67" width="18.37890625" customWidth="true"/>
-    <col min="68" max="68" width="17.7109375" customWidth="true"/>
-    <col min="69" max="69" width="17.93359375" customWidth="true"/>
-    <col min="70" max="70" width="18.046875" customWidth="true"/>
-    <col min="71" max="71" width="18.82421875" customWidth="true"/>
-    <col min="72" max="72" width="19.046875" customWidth="true"/>
-    <col min="73" max="73" width="16.7109375" customWidth="true"/>
-    <col min="74" max="74" width="16.93359375" customWidth="true"/>
-    <col min="75" max="75" width="16.26953125" customWidth="true"/>
-    <col min="76" max="76" width="16.48828125" customWidth="true"/>
-    <col min="77" max="77" width="20.82421875" customWidth="true"/>
-    <col min="78" max="78" width="21.046875" customWidth="true"/>
-    <col min="79" max="79" width="17.82421875" customWidth="true"/>
-    <col min="80" max="80" width="18.046875" customWidth="true"/>
-    <col min="81" max="81" width="16.046875" customWidth="true"/>
-    <col min="82" max="82" width="16.26953125" customWidth="true"/>
-    <col min="83" max="83" width="17.15625" customWidth="true"/>
-    <col min="84" max="84" width="17.37890625" customWidth="true"/>
-    <col min="85" max="85" width="15.7109375" customWidth="true"/>
-    <col min="86" max="86" width="15.93359375" customWidth="true"/>
-    <col min="87" max="87" width="16.82421875" customWidth="true"/>
-    <col min="88" max="88" width="17.046875" customWidth="true"/>
-    <col min="89" max="89" width="23.37890625" customWidth="true"/>
-    <col min="90" max="90" width="23.6015625" customWidth="true"/>
-    <col min="91" max="91" width="24.48828125" customWidth="true"/>
-    <col min="92" max="92" width="24.7109375" customWidth="true"/>
-    <col min="93" max="93" width="23.046875" customWidth="true"/>
-    <col min="94" max="94" width="23.26953125" customWidth="true"/>
-    <col min="95" max="95" width="24.15625" customWidth="true"/>
-    <col min="96" max="96" width="24.37890625" customWidth="true"/>
-    <col min="97" max="97" width="27.15625" customWidth="true"/>
-    <col min="98" max="98" width="27.37890625" customWidth="true"/>
-    <col min="99" max="99" width="28.26953125" customWidth="true"/>
-    <col min="100" max="100" width="28.48828125" customWidth="true"/>
-    <col min="101" max="101" width="26.82421875" customWidth="true"/>
-    <col min="102" max="102" width="27.046875" customWidth="true"/>
-    <col min="103" max="103" width="27.93359375" customWidth="true"/>
-    <col min="104" max="104" width="28.15625" customWidth="true"/>
+    <col min="3" max="3" width="9.5703125" customWidth="true"/>
+    <col min="4" max="4" width="7.85546875" customWidth="true"/>
+    <col min="5" max="5" width="32.42578125" customWidth="true"/>
+    <col min="6" max="6" width="32.7109375" customWidth="true"/>
+    <col min="7" max="7" width="32" customWidth="true"/>
+    <col min="8" max="8" width="32.28515625" customWidth="true"/>
+    <col min="9" max="9" width="32.5703125" customWidth="true"/>
+    <col min="10" max="10" width="33.140625" customWidth="true"/>
+    <col min="11" max="11" width="33.42578125" customWidth="true"/>
+    <col min="12" max="12" width="30.85546875" customWidth="true"/>
+    <col min="13" max="13" width="31.140625" customWidth="true"/>
+    <col min="14" max="14" width="30.42578125" customWidth="true"/>
+    <col min="15" max="15" width="30.7109375" customWidth="true"/>
+    <col min="16" max="16" width="35.42578125" customWidth="true"/>
+    <col min="17" max="17" width="35.7109375" customWidth="true"/>
+    <col min="18" max="18" width="32" customWidth="true"/>
+    <col min="19" max="19" width="32.28515625" customWidth="true"/>
+    <col min="20" max="20" width="31.5703125" customWidth="true"/>
+    <col min="21" max="21" width="31.85546875" customWidth="true"/>
+    <col min="22" max="22" width="31.140625" customWidth="true"/>
+    <col min="23" max="23" width="31.42578125" customWidth="true"/>
+    <col min="24" max="24" width="31.7109375" customWidth="true"/>
+    <col min="25" max="25" width="32.28515625" customWidth="true"/>
+    <col min="26" max="26" width="32.5703125" customWidth="true"/>
+    <col min="27" max="27" width="30" customWidth="true"/>
+    <col min="28" max="28" width="30.28515625" customWidth="true"/>
+    <col min="29" max="29" width="29.5703125" customWidth="true"/>
+    <col min="30" max="30" width="29.85546875" customWidth="true"/>
+    <col min="31" max="31" width="34.5703125" customWidth="true"/>
+    <col min="32" max="32" width="34.85546875" customWidth="true"/>
+    <col min="33" max="33" width="31.140625" customWidth="true"/>
+    <col min="34" max="34" width="31.42578125" customWidth="true"/>
+    <col min="35" max="35" width="17.7109375" customWidth="true"/>
+    <col min="36" max="36" width="18" customWidth="true"/>
+    <col min="37" max="37" width="19.140625" customWidth="true"/>
+    <col min="38" max="38" width="19.42578125" customWidth="true"/>
+    <col min="39" max="39" width="19.140625" customWidth="true"/>
+    <col min="40" max="40" width="19.42578125" customWidth="true"/>
+    <col min="41" max="41" width="21.5703125" customWidth="true"/>
+    <col min="42" max="42" width="21.85546875" customWidth="true"/>
+    <col min="43" max="43" width="17.42578125" customWidth="true"/>
+    <col min="44" max="44" width="17.7109375" customWidth="true"/>
+    <col min="45" max="45" width="18.85546875" customWidth="true"/>
+    <col min="46" max="46" width="19.140625" customWidth="true"/>
+    <col min="47" max="47" width="18.85546875" customWidth="true"/>
+    <col min="48" max="48" width="19.140625" customWidth="true"/>
+    <col min="49" max="49" width="21.28515625" customWidth="true"/>
+    <col min="50" max="50" width="21.5703125" customWidth="true"/>
+    <col min="51" max="51" width="21.85546875" customWidth="true"/>
+    <col min="52" max="52" width="22.140625" customWidth="true"/>
+    <col min="53" max="53" width="21.42578125" customWidth="true"/>
+    <col min="54" max="54" width="21.7109375" customWidth="true"/>
+    <col min="55" max="55" width="22" customWidth="true"/>
+    <col min="56" max="56" width="22.5703125" customWidth="true"/>
+    <col min="57" max="57" width="22.85546875" customWidth="true"/>
+    <col min="58" max="58" width="20.28515625" customWidth="true"/>
+    <col min="59" max="59" width="20.5703125" customWidth="true"/>
+    <col min="60" max="60" width="19.85546875" customWidth="true"/>
+    <col min="61" max="61" width="20.140625" customWidth="true"/>
+    <col min="62" max="62" width="24.85546875" customWidth="true"/>
+    <col min="63" max="63" width="25.140625" customWidth="true"/>
+    <col min="64" max="64" width="21.42578125" customWidth="true"/>
+    <col min="65" max="65" width="21.7109375" customWidth="true"/>
+    <col min="66" max="66" width="19.5703125" customWidth="true"/>
+    <col min="67" max="67" width="19.85546875" customWidth="true"/>
+    <col min="68" max="68" width="19.140625" customWidth="true"/>
+    <col min="69" max="69" width="19.42578125" customWidth="true"/>
+    <col min="70" max="70" width="19.7109375" customWidth="true"/>
+    <col min="71" max="71" width="20.28515625" customWidth="true"/>
+    <col min="72" max="72" width="20.5703125" customWidth="true"/>
+    <col min="73" max="73" width="18" customWidth="true"/>
+    <col min="74" max="74" width="18.28515625" customWidth="true"/>
+    <col min="75" max="75" width="17.5703125" customWidth="true"/>
+    <col min="76" max="76" width="17.85546875" customWidth="true"/>
+    <col min="77" max="77" width="22.5703125" customWidth="true"/>
+    <col min="78" max="78" width="22.85546875" customWidth="true"/>
+    <col min="79" max="79" width="19.140625" customWidth="true"/>
+    <col min="80" max="80" width="19.42578125" customWidth="true"/>
+    <col min="81" max="81" width="17.28515625" customWidth="true"/>
+    <col min="82" max="82" width="17.5703125" customWidth="true"/>
+    <col min="83" max="83" width="18.42578125" customWidth="true"/>
+    <col min="84" max="84" width="18.7109375" customWidth="true"/>
+    <col min="85" max="85" width="17" customWidth="true"/>
+    <col min="86" max="86" width="17.28515625" customWidth="true"/>
+    <col min="87" max="87" width="18.140625" customWidth="true"/>
+    <col min="88" max="88" width="18.42578125" customWidth="true"/>
+    <col min="89" max="89" width="25.28515625" customWidth="true"/>
+    <col min="90" max="90" width="25.5703125" customWidth="true"/>
+    <col min="91" max="91" width="26.42578125" customWidth="true"/>
+    <col min="92" max="92" width="26.7109375" customWidth="true"/>
+    <col min="93" max="93" width="25" customWidth="true"/>
+    <col min="94" max="94" width="25.28515625" customWidth="true"/>
+    <col min="95" max="95" width="26.140625" customWidth="true"/>
+    <col min="96" max="96" width="26.42578125" customWidth="true"/>
+    <col min="97" max="97" width="29.140625" customWidth="true"/>
+    <col min="98" max="98" width="29.42578125" customWidth="true"/>
+    <col min="99" max="99" width="30.28515625" customWidth="true"/>
+    <col min="100" max="100" width="30.5703125" customWidth="true"/>
+    <col min="101" max="101" width="28.85546875" customWidth="true"/>
+    <col min="102" max="102" width="29.140625" customWidth="true"/>
+    <col min="103" max="103" width="30" customWidth="true"/>
+    <col min="104" max="104" width="30.28515625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>914</v>
+        <v>1095</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>992</v>
+        <v>1173</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>993</v>
+        <v>1174</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>994</v>
+        <v>1175</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>995</v>
+        <v>1176</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>996</v>
+        <v>1177</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>997</v>
+        <v>1178</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>998</v>
+        <v>1179</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>999</v>
+        <v>1180</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1000</v>
+        <v>1181</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1001</v>
+        <v>1182</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1002</v>
+        <v>1183</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1003</v>
+        <v>1184</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1004</v>
+        <v>1185</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1005</v>
+        <v>1186</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1006</v>
+        <v>1187</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>1007</v>
+        <v>1188</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>1008</v>
+        <v>1189</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>1009</v>
+        <v>1190</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>1010</v>
+        <v>1191</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>1011</v>
+        <v>1192</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>1012</v>
+        <v>1193</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>1013</v>
+        <v>1194</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>1014</v>
+        <v>1195</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>1015</v>
+        <v>1196</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>1016</v>
+        <v>1197</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>1017</v>
+        <v>1198</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>1018</v>
+        <v>1199</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>1019</v>
+        <v>1200</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>1020</v>
+        <v>1201</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>1021</v>
+        <v>1202</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>1022</v>
+        <v>1203</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>1023</v>
+        <v>1204</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>1024</v>
+        <v>1205</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>1025</v>
+        <v>1206</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>1026</v>
+        <v>1207</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>1027</v>
+        <v>1208</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>1028</v>
+        <v>1209</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>1029</v>
+        <v>1210</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>1030</v>
+        <v>1211</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>1031</v>
+        <v>1212</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>1032</v>
+        <v>1213</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>1033</v>
+        <v>1214</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>1034</v>
+        <v>1215</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>1035</v>
+        <v>1216</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>1036</v>
+        <v>1217</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>1037</v>
+        <v>1218</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>1038</v>
+        <v>1219</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>1039</v>
+        <v>1220</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>1040</v>
+        <v>1221</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>1041</v>
+        <v>1222</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>1042</v>
+        <v>1223</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>1043</v>
+        <v>1224</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>1044</v>
+        <v>1225</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>1045</v>
+        <v>1226</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>1046</v>
+        <v>1227</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>1047</v>
+        <v>1228</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>1048</v>
+        <v>1229</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>1049</v>
+        <v>1230</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>1050</v>
+        <v>1231</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>1051</v>
+        <v>1232</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>1052</v>
+        <v>1233</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>1053</v>
+        <v>1234</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>1054</v>
+        <v>1235</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>1055</v>
+        <v>1236</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>1056</v>
+        <v>1237</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>1057</v>
+        <v>1238</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>1058</v>
+        <v>1239</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>1059</v>
+        <v>1240</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>1060</v>
+        <v>1241</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>1061</v>
+        <v>1242</v>
       </c>
       <c r="BT1" s="0" t="s">
-        <v>1062</v>
+        <v>1243</v>
       </c>
       <c r="BU1" s="0" t="s">
-        <v>1063</v>
+        <v>1244</v>
       </c>
       <c r="BV1" s="0" t="s">
-        <v>1064</v>
+        <v>1245</v>
       </c>
       <c r="BW1" s="0" t="s">
-        <v>1065</v>
+        <v>1246</v>
       </c>
       <c r="BX1" s="0" t="s">
-        <v>1066</v>
+        <v>1247</v>
       </c>
       <c r="BY1" s="0" t="s">
-        <v>1067</v>
+        <v>1248</v>
       </c>
       <c r="BZ1" s="0" t="s">
-        <v>1068</v>
+        <v>1249</v>
       </c>
       <c r="CA1" s="0" t="s">
-        <v>1069</v>
+        <v>1250</v>
       </c>
       <c r="CB1" s="0" t="s">
-        <v>1070</v>
+        <v>1251</v>
       </c>
       <c r="CC1" s="0" t="s">
-        <v>1071</v>
+        <v>1252</v>
       </c>
       <c r="CD1" s="0" t="s">
-        <v>1072</v>
+        <v>1253</v>
       </c>
       <c r="CE1" s="0" t="s">
-        <v>1073</v>
+        <v>1254</v>
       </c>
       <c r="CF1" s="0" t="s">
-        <v>1074</v>
+        <v>1255</v>
       </c>
       <c r="CG1" s="0" t="s">
-        <v>1075</v>
+        <v>1256</v>
       </c>
       <c r="CH1" s="0" t="s">
-        <v>1076</v>
+        <v>1257</v>
       </c>
       <c r="CI1" s="0" t="s">
-        <v>1077</v>
+        <v>1258</v>
       </c>
       <c r="CJ1" s="0" t="s">
-        <v>1078</v>
+        <v>1259</v>
       </c>
       <c r="CK1" s="0" t="s">
-        <v>1079</v>
+        <v>1260</v>
       </c>
       <c r="CL1" s="0" t="s">
-        <v>1080</v>
+        <v>1261</v>
       </c>
       <c r="CM1" s="0" t="s">
-        <v>1081</v>
+        <v>1262</v>
       </c>
       <c r="CN1" s="0" t="s">
-        <v>1082</v>
+        <v>1263</v>
       </c>
       <c r="CO1" s="0" t="s">
-        <v>1083</v>
+        <v>1264</v>
       </c>
       <c r="CP1" s="0" t="s">
-        <v>1084</v>
+        <v>1265</v>
       </c>
       <c r="CQ1" s="0" t="s">
-        <v>1085</v>
+        <v>1266</v>
       </c>
       <c r="CR1" s="0" t="s">
-        <v>1086</v>
+        <v>1267</v>
       </c>
       <c r="CS1" s="0" t="s">
-        <v>1087</v>
+        <v>1268</v>
       </c>
       <c r="CT1" s="0" t="s">
-        <v>1088</v>
+        <v>1269</v>
       </c>
       <c r="CU1" s="0" t="s">
-        <v>1089</v>
+        <v>1270</v>
       </c>
       <c r="CV1" s="0" t="s">
-        <v>1090</v>
+        <v>1271</v>
       </c>
       <c r="CW1" s="0" t="s">
-        <v>1091</v>
+        <v>1272</v>
       </c>
       <c r="CX1" s="0" t="s">
-        <v>1092</v>
+        <v>1273</v>
       </c>
       <c r="CY1" s="0" t="s">
-        <v>1093</v>
+        <v>1274</v>
       </c>
       <c r="CZ1" s="0" t="s">
-        <v>1094</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>915</v>
+        <v>1096</v>
       </c>
       <c r="B2" s="0">
         <v>9.6999999999999993</v>
@@ -4094,7 +4639,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>916</v>
+        <v>1097</v>
       </c>
       <c r="B3" s="0">
         <v>9.8734999999999999</v>
@@ -4408,7 +4953,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>917</v>
+        <v>1098</v>
       </c>
       <c r="B4" s="0">
         <v>9.7708333333333339</v>
@@ -4722,7 +5267,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>918</v>
+        <v>1099</v>
       </c>
       <c r="B5" s="0">
         <v>9.8226666666666667</v>
@@ -5036,7 +5581,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>919</v>
+        <v>1100</v>
       </c>
       <c r="B6" s="0">
         <v>9.7533333333333339</v>
@@ -5350,7 +5895,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>920</v>
+        <v>1101</v>
       </c>
       <c r="B7" s="0">
         <v>9.7533333333333339</v>
@@ -5664,7 +6209,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>921</v>
+        <v>1102</v>
       </c>
       <c r="B8" s="0">
         <v>9.7125000000000004</v>
@@ -5978,7 +6523,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>922</v>
+        <v>1103</v>
       </c>
       <c r="B9" s="0">
         <v>9.75</v>
@@ -6292,7 +6837,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>923</v>
+        <v>1104</v>
       </c>
       <c r="B10" s="0">
         <v>9.7166666666666668</v>
@@ -6606,7 +7151,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>924</v>
+        <v>1105</v>
       </c>
       <c r="B11" s="0">
         <v>9.7410000000000014</v>
@@ -6920,7 +7465,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>925</v>
+        <v>1106</v>
       </c>
       <c r="B12" s="0">
         <v>22.573666666666668</v>
@@ -7234,7 +7779,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>926</v>
+        <v>1107</v>
       </c>
       <c r="B13" s="0">
         <v>9.8641666666666676</v>
@@ -7548,7 +8093,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>927</v>
+        <v>1108</v>
       </c>
       <c r="B14" s="0">
         <v>9.9124999999999996</v>
@@ -7862,7 +8407,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>928</v>
+        <v>1109</v>
       </c>
       <c r="B15" s="0">
         <v>30.07</v>
@@ -8176,7 +8721,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>929</v>
+        <v>1110</v>
       </c>
       <c r="B16" s="0">
         <v>23.881666666666668</v>
@@ -8490,7 +9035,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>930</v>
+        <v>1111</v>
       </c>
       <c r="B17" s="0">
         <v>19.949999999999999</v>
@@ -8800,7 +9345,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>931</v>
+        <v>1112</v>
       </c>
       <c r="B18" s="0">
         <v>9.7183333333333337</v>
@@ -9114,7 +9659,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>932</v>
+        <v>1113</v>
       </c>
       <c r="B19" s="0">
         <v>9.7183333333333337</v>
@@ -9428,7 +9973,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>933</v>
+        <v>1114</v>
       </c>
       <c r="B20" s="0">
         <v>9.7400000000000002</v>
@@ -9742,7 +10287,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>934</v>
+        <v>1115</v>
       </c>
       <c r="B21" s="0">
         <v>9.7400000000000002</v>
@@ -10056,7 +10601,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>935</v>
+        <v>1116</v>
       </c>
       <c r="B22" s="0">
         <v>19.5</v>
@@ -10370,7 +10915,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>936</v>
+        <v>1117</v>
       </c>
       <c r="B23" s="0">
         <v>14.688000000000001</v>
@@ -10684,7 +11229,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>937</v>
+        <v>1118</v>
       </c>
       <c r="B24" s="0">
         <v>24.862500000000001</v>
@@ -10998,7 +11543,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>938</v>
+        <v>1119</v>
       </c>
       <c r="B25" s="0">
         <v>23.705666666666666</v>
@@ -11312,7 +11857,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>939</v>
+        <v>1120</v>
       </c>
       <c r="B26" s="0">
         <v>19.824999999999999</v>
@@ -11626,7 +12171,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>940</v>
+        <v>1121</v>
       </c>
       <c r="B27" s="0">
         <v>7.7208333333333332</v>
@@ -11940,7 +12485,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>941</v>
+        <v>1122</v>
       </c>
       <c r="B28" s="0">
         <v>12.330333333333334</v>
@@ -12254,7 +12799,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>942</v>
+        <v>1123</v>
       </c>
       <c r="B29" s="0">
         <v>29.984500000000001</v>
@@ -12568,7 +13113,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>943</v>
+        <v>1124</v>
       </c>
       <c r="B30" s="0">
         <v>9.75</v>
@@ -12882,7 +13427,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>944</v>
+        <v>1125</v>
       </c>
       <c r="B31" s="0">
         <v>9.706666666666667</v>
@@ -13196,7 +13741,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>945</v>
+        <v>1126</v>
       </c>
       <c r="B32" s="0">
         <v>9.7166666666666668</v>
@@ -13510,7 +14055,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>946</v>
+        <v>1127</v>
       </c>
       <c r="B33" s="0">
         <v>9.9616666666666678</v>
@@ -13824,7 +14369,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>947</v>
+        <v>1128</v>
       </c>
       <c r="B34" s="0">
         <v>9.6999999999999993</v>
@@ -14138,7 +14683,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>948</v>
+        <v>1129</v>
       </c>
       <c r="B35" s="0">
         <v>9.7370000000000001</v>
@@ -14452,7 +14997,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>949</v>
+        <v>1130</v>
       </c>
       <c r="B36" s="0">
         <v>9.7191666666666663</v>
@@ -14766,7 +15311,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>950</v>
+        <v>1131</v>
       </c>
       <c r="B37" s="0">
         <v>9.7386666666666653</v>
@@ -15080,7 +15625,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>951</v>
+        <v>1132</v>
       </c>
       <c r="B38" s="0">
         <v>23.913166666666665</v>
@@ -15394,7 +15939,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>952</v>
+        <v>1133</v>
       </c>
       <c r="B39" s="0">
         <v>19.885000000000002</v>
@@ -15708,7 +16253,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>953</v>
+        <v>1134</v>
       </c>
       <c r="B40" s="0">
         <v>9.8883333333333336</v>
@@ -16022,7 +16567,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>954</v>
+        <v>1135</v>
       </c>
       <c r="B41" s="0">
         <v>9.8938333333333333</v>
@@ -16336,7 +16881,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>955</v>
+        <v>1136</v>
       </c>
       <c r="B42" s="0">
         <v>19.782</v>
@@ -16650,7 +17195,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>956</v>
+        <v>1137</v>
       </c>
       <c r="B43" s="0">
         <v>19.885000000000002</v>
@@ -16964,7 +17509,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>957</v>
+        <v>1138</v>
       </c>
       <c r="B44" s="0">
         <v>9.8666666666666671</v>
@@ -17278,7 +17823,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>958</v>
+        <v>1139</v>
       </c>
       <c r="B45" s="0">
         <v>9.8940000000000001</v>
@@ -17592,7 +18137,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>959</v>
+        <v>1140</v>
       </c>
       <c r="B46" s="0">
         <v>14.699999999999999</v>
@@ -17906,7 +18451,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>960</v>
+        <v>1141</v>
       </c>
       <c r="B47" s="0">
         <v>9.8940000000000001</v>
@@ -18220,7 +18765,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>961</v>
+        <v>1142</v>
       </c>
       <c r="B48" s="0">
         <v>9.8449999999999989</v>
@@ -18534,7 +19079,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>962</v>
+        <v>1143</v>
       </c>
       <c r="B49" s="0">
         <v>9.8536666666666672</v>
@@ -18848,7 +19393,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>963</v>
+        <v>1144</v>
       </c>
       <c r="B50" s="0">
         <v>9.9449999999999985</v>
@@ -19162,7 +19707,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>964</v>
+        <v>1145</v>
       </c>
       <c r="B51" s="0">
         <v>19.895</v>
@@ -19476,7 +20021,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>965</v>
+        <v>1146</v>
       </c>
       <c r="B52" s="0">
         <v>9.9013333333333335</v>
@@ -19790,7 +20335,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>966</v>
+        <v>1147</v>
       </c>
       <c r="B53" s="0">
         <v>9.8820000000000014</v>
@@ -20104,7 +20649,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>967</v>
+        <v>1148</v>
       </c>
       <c r="B54" s="0">
         <v>9.9449999999999985</v>
@@ -20418,7 +20963,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>968</v>
+        <v>1149</v>
       </c>
       <c r="B55" s="0">
         <v>9.9000000000000004</v>
@@ -20732,7 +21277,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>969</v>
+        <v>1150</v>
       </c>
       <c r="B56" s="0">
         <v>9.9000000000000004</v>
@@ -21046,7 +21591,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>970</v>
+        <v>1151</v>
       </c>
       <c r="B57" s="0">
         <v>9.8175000000000008</v>
@@ -21360,7 +21905,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>971</v>
+        <v>1152</v>
       </c>
       <c r="B58" s="0">
         <v>9.8533333333333317</v>
@@ -21674,7 +22219,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>972</v>
+        <v>1153</v>
       </c>
       <c r="B59" s="0">
         <v>29.949000000000002</v>
@@ -21988,7 +22533,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>973</v>
+        <v>1154</v>
       </c>
       <c r="B60" s="0">
         <v>10.013333333333332</v>
@@ -22302,7 +22847,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>974</v>
+        <v>1155</v>
       </c>
       <c r="B61" s="0">
         <v>9.9013333333333335</v>
@@ -22616,7 +23161,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>975</v>
+        <v>1156</v>
       </c>
       <c r="B62" s="0">
         <v>9.8685000000000009</v>
@@ -22930,7 +23475,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>976</v>
+        <v>1157</v>
       </c>
       <c r="B63" s="0">
         <v>9.8933333333333326</v>
@@ -23244,7 +23789,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>977</v>
+        <v>1158</v>
       </c>
       <c r="B64" s="0">
         <v>9.9148333333333323</v>
@@ -23558,7 +24103,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>978</v>
+        <v>1159</v>
       </c>
       <c r="B65" s="0">
         <v>9.9513333333333343</v>
@@ -23872,7 +24417,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>979</v>
+        <v>1160</v>
       </c>
       <c r="B66" s="0">
         <v>9.9166666666666661</v>
@@ -24186,7 +24731,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>980</v>
+        <v>1161</v>
       </c>
       <c r="B67" s="0">
         <v>9.9324999999999992</v>
@@ -24500,7 +25045,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>981</v>
+        <v>1162</v>
       </c>
       <c r="B68" s="0">
         <v>19.933333333333334</v>
@@ -24814,7 +25359,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>982</v>
+        <v>1163</v>
       </c>
       <c r="B69" s="0">
         <v>19.920000000000002</v>
@@ -25128,7 +25673,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>983</v>
+        <v>1164</v>
       </c>
       <c r="B70" s="0">
         <v>9.8410000000000011</v>
@@ -25442,7 +25987,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>984</v>
+        <v>1165</v>
       </c>
       <c r="B71" s="0">
         <v>9.8410000000000011</v>
@@ -25756,7 +26301,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>985</v>
+        <v>1166</v>
       </c>
       <c r="B72" s="0">
         <v>29.973000000000003</v>
@@ -26070,7 +26615,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>986</v>
+        <v>1167</v>
       </c>
       <c r="B73" s="0">
         <v>9.9008333333333347</v>
@@ -26384,7 +26929,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>987</v>
+        <v>1168</v>
       </c>
       <c r="B74" s="0">
         <v>9.9000000000000004</v>
@@ -26698,7 +27243,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>988</v>
+        <v>1169</v>
       </c>
       <c r="B75" s="0">
         <v>9.8856666666666673</v>
@@ -27012,7 +27557,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>989</v>
+        <v>1170</v>
       </c>
       <c r="B76" s="0">
         <v>19.900833333333331</v>
@@ -27326,7 +27871,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>990</v>
+        <v>1171</v>
       </c>
       <c r="B77" s="0">
         <v>9.9169999999999998</v>
@@ -27640,7 +28185,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>991</v>
+        <v>1172</v>
       </c>
       <c r="B78" s="0">
         <v>9.9169999999999998</v>

</xml_diff>